<commit_message>
modified:   figures/figure 3.ipynb 	modified:   figures/gdp/gdp for eleven cities.xls 	new file:   figures/private_dental_clinics_by_city_and_year.png 	modified:   regression analysis/spregression_8_5.ipynb 	modified:   regression analysis/table 4.xlsx
</commit_message>
<xml_diff>
--- a/regression analysis/table 4.xlsx
+++ b/regression analysis/table 4.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2016-2019" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2020-2022" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="non-public" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="with-public" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1566,4 +1568,1152 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>betas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tval</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>pval</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0637088731313248</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>end_price_pers</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.02238315851785786</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.846286107498913</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.004423243349374988</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.7593975990057419</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1025429604858371</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.405653156567756</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.305065219678907e-13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01251956201842215</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>light</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.002784357840487596</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.496391173711252</v>
+      </c>
+      <c r="F4" t="n">
+        <v>6.9116529259573e-06</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.01077524367234719</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001653920264806647</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6.514971671628246</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7.27033777922428e-11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.03590023213760504</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>elect_store</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.007784953465750745</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-4.611489624895656</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.997936150470529e-06</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.08042991992061747</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.01170855419272161</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6.869329773492884</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6.450423702714271e-12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0009188494730057676</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.003505818216727482</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2620927316258487</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7932499502947528</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.09957865546870498</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>hotel_num</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.01872490744341301</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-5.317978514427019</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.049264555773517e-07</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0897335773351611</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>mall</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0100767496612824</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8.905012067526274</v>
+      </c>
+      <c r="F10" t="n">
+        <v>5.338024012456652e-19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0681412197591295</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>museum_num</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.03207401752967017</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.124499049615323</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.03362843543888307</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.06201438711410339</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>old</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.03361405766034116</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.844894411163867</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.06505289983273083</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.01886967576864667</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ktv</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.006952403994776279</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.714122450712658</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.006645159837183084</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.05759735098984133</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.02495306768315119</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.308227257714377</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0209864998688624</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.04044446848911891</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>primary</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.02384813478090232</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.695917473659492</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.08990151000025703</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.0007188371302023358</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>west_food</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.009316348107866395</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-0.07715868083496957</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9384973115290606</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.07676307722657912</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.01476243462578291</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5.199892780050705</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.994035203801389e-07</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.1971501125630096</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>green_ratio</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2171865486487065</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.9077455016880198</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.3640126977409962</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.001735985817913426</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>number_building</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.001487015025690822</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1.167429910203456</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.2430367980400935</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.05453573902918429</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>tihu</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1014216886986797</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.5377127883485363</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.5907753490410359</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.20222518177387</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sub</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.05122367266021394</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.947885250542388</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7.884457746141509e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.001203659398459148</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>floor_ratio</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.005907814001665293</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.2037402325326866</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.8385565005398621</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.793027881369573e-05</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>residence</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.237864787995816e-05</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.4230970007463445</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.6722244905542698</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1050286737796948</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>park</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.01611663819562338</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6.516785480002669</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7.183003569083262e-11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.3874334265550495</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>W_kou</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.01364562403362328</v>
+      </c>
+      <c r="E25" t="n">
+        <v>28.39250338426447</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.502484616927769e-177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>betas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tval</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>pval</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.04377605336263387</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>end_price_pers</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0.00564526274949352</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7.754475797705139</v>
+      </c>
+      <c r="F2" t="n">
+        <v>8.870913996172622e-15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.959082868500801</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>pop</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.04749848506487064</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20.19186227078489</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.154305096726273e-90</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.01073859511211014</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>light</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0008143977526359257</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.18593411800683</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.057361136058038e-39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.005749974025439229</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>pm25</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0004883022089631953</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-11.77544135556557</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5.224294340831422e-32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-0.06721149416600077</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>elect_store</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.005584747257481041</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-12.03483184954658</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.331084923773761e-33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.09619071195437488</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>kind</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.004008706111860803</v>
+      </c>
+      <c r="E7" t="n">
+        <v>23.99545121798018</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3.10210932730317e-127</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.005449340192978054</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001094841438308703</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.977287123326393</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6.448163618429017e-07</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.1202579828244073</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>hotel_num</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.009976158486020856</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-12.05453812636592</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.835585699084158e-33</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.05567348910636791</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>mall</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.00395080415821821</v>
+      </c>
+      <c r="E10" t="n">
+        <v>14.09168535741249</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4.272421689789468e-45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1303558675702017</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>museum_num</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0197488292065366</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6.60068838546923</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.092529716942461e-11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.05613176093359085</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>old</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01687623348327957</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.326083452756469</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0008807555450991296</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.01948603866213898</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ktv</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.003789171827270449</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.142558730617359</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2.710216776840407e-07</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0387479538324378</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0.01126137518572047</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.440783491661885</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0005800324588749407</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1081165504577916</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>primary</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.01083609246706428</v>
+      </c>
+      <c r="E15" t="n">
+        <v>9.977448124072955</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.913240165307493e-23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.01425896921789705</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>west_food</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.004593741965328372</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.103998728164911</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0019092415168455</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0861367748886903</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>super</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.006196877208041567</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.90002932072178</v>
+      </c>
+      <c r="F17" t="n">
+        <v>6.33154231032481e-44</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.4016180539608001</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>green_ratio</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.06294278770727448</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-6.380684246598502</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.762984750860955e-10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.0002944294891112696</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>number_building</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0001448205766837595</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-2.03306391849417</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.04204606572397063</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>-0.04206458033378282</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>tihu</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.01687667229857829</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-2.492468870022817</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.01268584503278715</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1840730562249867</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sub</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.02006160458153283</v>
+      </c>
+      <c r="E21" t="n">
+        <v>9.175390506621298</v>
+      </c>
+      <c r="F21" t="n">
+        <v>4.499406579171819e-20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>5.376666124485034e-05</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>floor_ratio</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0006539656863377688</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.08221633392715995</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.9344746848226322</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2.616653593235976e-06</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>residence</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>6.642911969326626e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.3939015909466009</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.693653695733659</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.08687055406353217</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>park</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.006052228618040066</v>
+      </c>
+      <c r="E24" t="n">
+        <v>14.35348192310423</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.01319875154469e-46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.3573186051384035</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>W_kou</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.005803869959308016</v>
+      </c>
+      <c r="E25" t="n">
+        <v>61.56557738950545</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>